<commit_message>
implement cam table for X/Y/Y/Theta axis
</commit_message>
<xml_diff>
--- a/plc_register_configuration.xlsx
+++ b/plc_register_configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WingTsui\Documents\github\Ebots_CTC_PLC_Program_Ecat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Denali\PLC_CTC\Ebots_CTC_PLC_Program_Ecat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{410047F5-7BFF-4915-A6AB-71FB9E5E25BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D840440-6835-4BDA-82CB-BEB8E4D81442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -24,90 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Wing Tsui</author>
-  </authors>
-  <commentList>
-    <comment ref="B81" authorId="0" shapeId="0" xr:uid="{41786475-7099-4722-AF40-0479E3E719EF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Wing Tsui:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-EmptyAxis1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B94" authorId="0" shapeId="0" xr:uid="{646156AC-B3D4-4218-96D4-8973359EED81}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Wing Tsui:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-EmptyAxis2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B120" authorId="0" shapeId="0" xr:uid="{85158EEA-6E0A-4126-BD68-D026DD78083C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Wing Tsui:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-AxisEmpty3</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="54">
   <si>
     <t>Axis1</t>
   </si>
@@ -163,36 +81,78 @@
     <t>PLC Outputs</t>
   </si>
   <si>
+    <t>PhoneClampClosed</t>
+  </si>
+  <si>
+    <t>PhoneClampOpen</t>
+  </si>
+  <si>
+    <t>TransferStationClampOpen</t>
+  </si>
+  <si>
     <t>Feedback Position (R only)</t>
   </si>
   <si>
+    <t>TransferStationClampClosed</t>
+  </si>
+  <si>
+    <t>RollerExtension</t>
+  </si>
+  <si>
     <t>Motion Commands :  1=Go : 3=JogCW : 4=JogCCW : 5=Home : 0=STOP  : 6=DriveDisable :  7=DriveEnable</t>
   </si>
   <si>
+    <t>RollerRetraction</t>
+  </si>
+  <si>
+    <t>GripperClose</t>
+  </si>
+  <si>
+    <t>OutsidePlugnerDown</t>
+  </si>
+  <si>
     <t>Axis3</t>
   </si>
   <si>
     <t>Stage Axis Z</t>
   </si>
   <si>
+    <t>GripperOpen</t>
+  </si>
+  <si>
+    <t>OutsidePlugnerUp</t>
+  </si>
+  <si>
+    <t>PhoneSuctionSupply</t>
+  </si>
+  <si>
+    <t>PhoneSuctionBlowoff</t>
+  </si>
+  <si>
+    <t>InsidePlugnerDown</t>
+  </si>
+  <si>
+    <t>InsidePlugnerUp</t>
+  </si>
+  <si>
+    <t>Axis4</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>Axis5</t>
+  </si>
+  <si>
+    <t>Gripper</t>
+  </si>
+  <si>
     <t>Statas</t>
   </si>
   <si>
     <t>EtherCAT</t>
   </si>
   <si>
-    <t>Axis4</t>
-  </si>
-  <si>
-    <t>Theta</t>
-  </si>
-  <si>
-    <t>Axis5</t>
-  </si>
-  <si>
-    <t>Gripper</t>
-  </si>
-  <si>
     <t>Axis6</t>
   </si>
   <si>
@@ -221,31 +181,24 @@
   </si>
   <si>
     <t>IrisCup</t>
+  </si>
+  <si>
+    <t>Motion command:   1=Go : 3=JogCW : 4=JogCCW : 5=Home : 0=STOP  : 6=DriveDisable :  7=DriveEnable : 9= SetFeedback : 10=3D Motion : 13=CamMotion</t>
+  </si>
+  <si>
+    <t>Axis - broadcast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -269,8 +222,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,33 +540,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="31.33203125"/>
-    <col min="2" max="2" width="25.5546875"/>
-    <col min="3" max="3" width="12.5546875"/>
-    <col min="4" max="4" width="20.21875"/>
-    <col min="5" max="5" width="20.109375"/>
-    <col min="6" max="6" width="8.5546875"/>
-    <col min="7" max="7" width="11.6640625"/>
-    <col min="8" max="8" width="12.5546875"/>
-    <col min="9" max="9" width="20.21875"/>
-    <col min="10" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="31.3671875" customWidth="1"/>
+    <col min="2" max="2" width="25.578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5234375" customWidth="1"/>
+    <col min="4" max="4" width="20.26171875" customWidth="1"/>
+    <col min="5" max="5" width="20.15625" customWidth="1"/>
+    <col min="6" max="6" width="8.578125" customWidth="1"/>
+    <col min="7" max="7" width="11.68359375" customWidth="1"/>
+    <col min="8" max="8" width="12.5234375" customWidth="1"/>
+    <col min="9" max="9" width="20.26171875" customWidth="1"/>
+    <col min="10" max="10" width="18.9453125" customWidth="1"/>
+    <col min="11" max="1025" width="8.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -636,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -659,7 +616,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -682,7 +639,7 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -705,7 +662,7 @@
         <v>4004</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -728,7 +685,7 @@
         <v>4006</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -751,7 +708,7 @@
         <v>4008</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -774,7 +731,7 @@
         <v>4010</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -797,7 +754,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -820,7 +777,7 @@
         <v>4014</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -843,7 +800,7 @@
         <v>4016</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -866,7 +823,7 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -880,7 +837,7 @@
         <v>4020</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G15">
         <v>12</v>
       </c>
@@ -891,7 +848,7 @@
         <v>4022</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -917,7 +874,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -940,7 +897,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -963,7 +920,7 @@
         <v>4028</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -986,7 +943,7 @@
         <v>4030</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +957,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1045,8 +1002,11 @@
       <c r="I22">
         <v>2000</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -1068,8 +1028,11 @@
       <c r="I23">
         <v>2002</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -1091,10 +1054,13 @@
       <c r="I24">
         <v>2004</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>519</v>
@@ -1114,8 +1080,11 @@
       <c r="I25">
         <v>2006</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>13</v>
       </c>
@@ -1137,10 +1106,13 @@
       <c r="I26">
         <v>2008</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G27">
         <v>6</v>
@@ -1151,8 +1123,11 @@
       <c r="I27">
         <v>2010</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G28">
         <v>7</v>
       </c>
@@ -1162,13 +1137,19 @@
       <c r="I28">
         <v>2012</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1188,8 +1169,14 @@
       <c r="I29">
         <v>2014</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1211,8 +1198,11 @@
       <c r="I30">
         <v>2016</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -1234,8 +1224,11 @@
       <c r="I31">
         <v>2018</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>8</v>
       </c>
@@ -1257,8 +1250,11 @@
       <c r="I32">
         <v>2020</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -1280,8 +1276,11 @@
       <c r="I33">
         <v>2022</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" t="s">
         <v>11</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" t="s">
         <v>11</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" t="s">
         <v>11</v>
       </c>
@@ -1373,9 +1372,9 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C38">
         <v>529</v>
@@ -1387,7 +1386,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" t="s">
         <v>13</v>
       </c>
@@ -1401,7 +1400,7 @@
         <v>1059</v>
       </c>
       <c r="G39" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H39" t="s">
         <v>2</v>
@@ -1410,26 +1409,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
       </c>
       <c r="H40">
-        <v>13464</v>
+        <v>1017</v>
       </c>
       <c r="I40">
-        <v>26926</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2000</v>
+      </c>
+      <c r="J40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>1018</v>
+      </c>
+      <c r="I41">
+        <v>2002</v>
+      </c>
+      <c r="J41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -1440,8 +1456,20 @@
       <c r="E42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>1019</v>
+      </c>
+      <c r="I42">
+        <v>2004</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -1454,8 +1482,20 @@
       <c r="E43">
         <v>1061</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43">
+        <v>1020</v>
+      </c>
+      <c r="I43">
+        <v>2006</v>
+      </c>
+      <c r="J43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" t="s">
         <v>7</v>
       </c>
@@ -1468,8 +1508,17 @@
       <c r="E44">
         <v>1063</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44">
+        <v>1021</v>
+      </c>
+      <c r="I44">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" t="s">
         <v>8</v>
       </c>
@@ -1482,8 +1531,17 @@
       <c r="E45">
         <v>1065</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>6</v>
+      </c>
+      <c r="H45">
+        <v>1022</v>
+      </c>
+      <c r="I45">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" t="s">
         <v>9</v>
       </c>
@@ -1496,8 +1554,17 @@
       <c r="E46">
         <v>1067</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="H46">
+        <v>1023</v>
+      </c>
+      <c r="I46">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" t="s">
         <v>10</v>
       </c>
@@ -1510,8 +1577,17 @@
       <c r="E47">
         <v>1069</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>1024</v>
+      </c>
+      <c r="I47">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
         <v>11</v>
       </c>
@@ -1524,8 +1600,17 @@
       <c r="E48">
         <v>1071</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <v>1025</v>
+      </c>
+      <c r="I48">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
         <v>11</v>
       </c>
@@ -1538,8 +1623,17 @@
       <c r="E49">
         <v>1073</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>10</v>
+      </c>
+      <c r="H49">
+        <v>1026</v>
+      </c>
+      <c r="I49">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" t="s">
         <v>11</v>
       </c>
@@ -1552,10 +1646,19 @@
       <c r="E50">
         <v>1075</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>11</v>
+      </c>
+      <c r="H50">
+        <v>1027</v>
+      </c>
+      <c r="I50">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C51">
         <v>539</v>
@@ -1566,8 +1669,17 @@
       <c r="E51">
         <v>1077</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>12</v>
+      </c>
+      <c r="H51">
+        <v>1028</v>
+      </c>
+      <c r="I51">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" t="s">
         <v>13</v>
       </c>
@@ -1580,18 +1692,47 @@
       <c r="E52">
         <v>1079</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>13</v>
+      </c>
+      <c r="H52">
+        <v>1029</v>
+      </c>
+      <c r="I52">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="G53">
+        <v>14</v>
+      </c>
+      <c r="H53">
+        <v>1030</v>
+      </c>
+      <c r="I53">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G54">
+        <v>15</v>
+      </c>
+      <c r="H54">
+        <v>1031</v>
+      </c>
+      <c r="I54">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -1602,8 +1743,17 @@
       <c r="E55" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>16</v>
+      </c>
+      <c r="H55">
+        <v>1032</v>
+      </c>
+      <c r="I55">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" t="s">
         <v>6</v>
       </c>
@@ -1617,7 +1767,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" t="s">
         <v>7</v>
       </c>
@@ -1631,7 +1781,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" t="s">
         <v>8</v>
       </c>
@@ -1645,7 +1795,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" t="s">
         <v>9</v>
       </c>
@@ -1659,7 +1809,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" t="s">
         <v>10</v>
       </c>
@@ -1673,7 +1823,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" t="s">
         <v>11</v>
       </c>
@@ -1687,7 +1837,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" t="s">
         <v>11</v>
       </c>
@@ -1701,7 +1851,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" t="s">
         <v>11</v>
       </c>
@@ -1715,9 +1865,9 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C64">
         <v>549</v>
@@ -1728,8 +1878,17 @@
       <c r="E64">
         <v>1097</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" t="s">
+        <v>2</v>
+      </c>
+      <c r="I64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" t="s">
         <v>13</v>
       </c>
@@ -1742,18 +1901,27 @@
       <c r="E65">
         <v>1099</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G65" t="s">
+        <v>41</v>
+      </c>
+      <c r="H65">
+        <v>13464</v>
+      </c>
+      <c r="I65">
+        <v>26926</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
@@ -1765,7 +1933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" t="s">
         <v>6</v>
       </c>
@@ -1779,7 +1947,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" t="s">
         <v>7</v>
       </c>
@@ -1793,7 +1961,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" t="s">
         <v>8</v>
       </c>
@@ -1807,7 +1975,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +1989,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +2003,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" t="s">
         <v>11</v>
       </c>
@@ -1849,7 +2017,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" t="s">
         <v>11</v>
       </c>
@@ -1863,7 +2031,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" t="s">
         <v>11</v>
       </c>
@@ -1877,9 +2045,9 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C77">
         <v>559</v>
@@ -1891,7 +2059,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" t="s">
         <v>13</v>
       </c>
@@ -1905,17 +2073,17 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
@@ -1927,7 +2095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" t="s">
         <v>6</v>
       </c>
@@ -1941,7 +2109,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" t="s">
         <v>7</v>
       </c>
@@ -1955,7 +2123,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" t="s">
         <v>8</v>
       </c>
@@ -1969,7 +2137,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" t="s">
         <v>9</v>
       </c>
@@ -1983,7 +2151,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B86" t="s">
         <v>10</v>
       </c>
@@ -1997,7 +2165,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" t="s">
         <v>11</v>
       </c>
@@ -2011,7 +2179,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" t="s">
         <v>11</v>
       </c>
@@ -2025,7 +2193,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B89" t="s">
         <v>11</v>
       </c>
@@ -2039,9 +2207,9 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B90" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C90">
         <v>569</v>
@@ -2053,7 +2221,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" t="s">
         <v>13</v>
       </c>
@@ -2067,17 +2235,17 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
@@ -2089,7 +2257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" t="s">
         <v>6</v>
       </c>
@@ -2103,7 +2271,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" t="s">
         <v>7</v>
       </c>
@@ -2117,7 +2285,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" t="s">
         <v>8</v>
       </c>
@@ -2131,7 +2299,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" t="s">
         <v>9</v>
       </c>
@@ -2145,7 +2313,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" t="s">
         <v>10</v>
       </c>
@@ -2159,7 +2327,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B100" t="s">
         <v>11</v>
       </c>
@@ -2173,7 +2341,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B101" t="s">
         <v>11</v>
       </c>
@@ -2187,7 +2355,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B102" t="s">
         <v>11</v>
       </c>
@@ -2201,9 +2369,9 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C103">
         <v>579</v>
@@ -2215,7 +2383,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" t="s">
         <v>13</v>
       </c>
@@ -2229,17 +2397,17 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B107" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C107" t="s">
         <v>2</v>
@@ -2251,7 +2419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B108" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2433,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" t="s">
         <v>7</v>
       </c>
@@ -2279,7 +2447,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B110" t="s">
         <v>8</v>
       </c>
@@ -2293,7 +2461,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" t="s">
         <v>9</v>
       </c>
@@ -2307,7 +2475,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B112" t="s">
         <v>10</v>
       </c>
@@ -2321,7 +2489,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B113" t="s">
         <v>11</v>
       </c>
@@ -2335,7 +2503,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +2517,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" t="s">
         <v>11</v>
       </c>
@@ -2363,9 +2531,9 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C116">
         <v>589</v>
@@ -2377,7 +2545,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" t="s">
         <v>13</v>
       </c>
@@ -2391,17 +2559,17 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B120" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C120" t="s">
         <v>2</v>
@@ -2413,7 +2581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" t="s">
         <v>6</v>
       </c>
@@ -2427,7 +2595,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B122" t="s">
         <v>7</v>
       </c>
@@ -2441,7 +2609,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B123" t="s">
         <v>8</v>
       </c>
@@ -2455,7 +2623,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B124" t="s">
         <v>9</v>
       </c>
@@ -2469,7 +2637,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B125" t="s">
         <v>10</v>
       </c>
@@ -2483,7 +2651,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B126" t="s">
         <v>11</v>
       </c>
@@ -2497,7 +2665,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B127" t="s">
         <v>11</v>
       </c>
@@ -2511,7 +2679,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" t="s">
         <v>11</v>
       </c>
@@ -2525,9 +2693,9 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B129" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C129">
         <v>599</v>
@@ -2539,7 +2707,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B130" t="s">
         <v>13</v>
       </c>
@@ -2553,18 +2721,53 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="s">
+        <v>53</v>
+      </c>
+      <c r="B133" t="s">
+        <v>51</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" t="s">
+        <v>3</v>
+      </c>
+      <c r="E133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134">
+        <v>700</v>
+      </c>
+      <c r="D134">
+        <v>1398</v>
+      </c>
+      <c r="E134">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>